<commit_message>
ajustes visualizações e tabela com dados
</commit_message>
<xml_diff>
--- a/backtesting/constraints.xlsx
+++ b/backtesting/constraints.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andre\OneDrive\Documentos\Github\quantamental-Dev_Wizards\backtesting\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Documents\GitHub\quantamental-Dev_Wizards\backtesting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81EAEF52-3549-445A-BF41-8AE965CC5F88}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90D69F31-FA0B-4341-8A24-E5C3887530DC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="23260" windowHeight="12580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -410,15 +410,15 @@
   <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="F3" sqref="A3:F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="9" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="9" width="12.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -450,7 +450,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>9</v>
       </c>

</xml_diff>